<commit_message>
updating new fields to student profile/info
</commit_message>
<xml_diff>
--- a/SAMPLE STUDENTS/sample_students.xlsx
+++ b/SAMPLE STUDENTS/sample_students.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CCJ_SYSTEM_PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CCJ_SYSTEM_PROJECT\SAMPLE STUDENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7554B9B-E730-456E-A605-CB891FDB09DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A2E73F8-5648-4EE8-BFC0-92E02BBEB11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="sample_students" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="96">
   <si>
     <t>student_id_number</t>
   </si>
@@ -79,6 +79,9 @@
     <t>guardian_contact</t>
   </si>
   <si>
+    <t>enrollment_status</t>
+  </si>
+  <si>
     <t>school_year</t>
   </si>
   <si>
@@ -115,9 +118,21 @@
     <t>Father 1</t>
   </si>
   <si>
+    <t>Mother 1</t>
+  </si>
+  <si>
+    <t>Guardian 1</t>
+  </si>
+  <si>
+    <t>Enrolled</t>
+  </si>
+  <si>
     <t>2022-2023</t>
   </si>
   <si>
+    <t>1ST</t>
+  </si>
+  <si>
     <t>Jane</t>
   </si>
   <si>
@@ -142,40 +157,58 @@
     <t>State B</t>
   </si>
   <si>
-    <t>Guardian 1</t>
+    <t>Father 2</t>
+  </si>
+  <si>
+    <t>Guardian 2</t>
+  </si>
+  <si>
+    <t>Not Enrolled</t>
+  </si>
+  <si>
+    <t>2023-2024</t>
+  </si>
+  <si>
+    <t>2ND</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>Purok 3</t>
+  </si>
+  <si>
+    <t>Third St</t>
+  </si>
+  <si>
+    <t>Barangay 3</t>
+  </si>
+  <si>
+    <t>City C</t>
+  </si>
+  <si>
+    <t>State C</t>
+  </si>
+  <si>
+    <t>Father 3</t>
+  </si>
+  <si>
+    <t>Mother 3</t>
   </si>
   <si>
     <t>2024-2025</t>
   </si>
   <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Johnson</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>Purok 3</t>
-  </si>
-  <si>
-    <t>Third St</t>
-  </si>
-  <si>
-    <t>Barangay 3</t>
-  </si>
-  <si>
-    <t>City C</t>
-  </si>
-  <si>
-    <t>State C</t>
-  </si>
-  <si>
-    <t>Mother 1</t>
+    <t>3RD</t>
   </si>
   <si>
     <t>Sarah</t>
@@ -202,7 +235,13 @@
     <t>State D</t>
   </si>
   <si>
-    <t>Father 2</t>
+    <t>Father 4</t>
+  </si>
+  <si>
+    <t>Guardian 3</t>
+  </si>
+  <si>
+    <t>4TH</t>
   </si>
   <si>
     <t>Alex</t>
@@ -229,7 +268,16 @@
     <t>State F</t>
   </si>
   <si>
-    <t>Father 4</t>
+    <t>Father 5</t>
+  </si>
+  <si>
+    <t>Guardian 4</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>GRADUATE</t>
   </si>
   <si>
     <t>Natalie</t>
@@ -256,25 +304,10 @@
     <t>State G</t>
   </si>
   <si>
-    <t>Father 5</t>
-  </si>
-  <si>
-    <t>2023-2024</t>
-  </si>
-  <si>
-    <t>1ST</t>
-  </si>
-  <si>
-    <t>2ND</t>
-  </si>
-  <si>
-    <t>3RD</t>
-  </si>
-  <si>
-    <t>4TH</t>
-  </si>
-  <si>
-    <t>GRADUATE</t>
+    <t>Father 6</t>
+  </si>
+  <si>
+    <t>Guardian 5</t>
   </si>
 </sst>
 </file>
@@ -1116,24 +1149,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1200,316 +1222,385 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023001</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1">
         <v>38353</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <v>123</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M2">
         <v>9123456789</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
       </c>
       <c r="Q2">
         <v>9123456701</v>
       </c>
+      <c r="R2">
+        <v>9123456710</v>
+      </c>
+      <c r="S2">
+        <v>9123456722</v>
+      </c>
       <c r="T2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="U2" t="s">
-        <v>80</v>
+        <v>35</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2023002</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F3" s="1">
         <v>38385</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H3">
         <v>456</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="M3">
         <v>9234567890</v>
       </c>
+      <c r="N3" t="s">
+        <v>45</v>
+      </c>
       <c r="P3" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="Q3">
+        <v>9123456781</v>
+      </c>
+      <c r="R3">
+        <v>9123456792</v>
       </c>
       <c r="S3">
-        <v>9123456722</v>
+        <v>9123456733</v>
       </c>
       <c r="T3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="U3" t="s">
-        <v>81</v>
+        <v>48</v>
+      </c>
+      <c r="V3" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023003</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1">
         <v>38414</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="H4">
         <v>789</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="M4">
         <v>9345678901</v>
       </c>
+      <c r="N4" t="s">
+        <v>59</v>
+      </c>
       <c r="O4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="Q4">
-        <v>9123456713</v>
+        <v>9123456790</v>
+      </c>
+      <c r="R4">
+        <v>9123456709</v>
       </c>
       <c r="T4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="U4" t="s">
-        <v>82</v>
+        <v>61</v>
+      </c>
+      <c r="V4" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2023004</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="F5" s="1">
         <v>38081</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="H5">
         <v>101</v>
       </c>
       <c r="I5" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="K5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="L5" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="M5">
         <v>9456789012</v>
       </c>
       <c r="N5" t="s">
-        <v>60</v>
+        <v>71</v>
+      </c>
+      <c r="P5" t="s">
+        <v>72</v>
       </c>
       <c r="Q5">
-        <v>9123456780</v>
+        <v>9123456708</v>
+      </c>
+      <c r="R5">
+        <v>9123456715</v>
+      </c>
+      <c r="S5">
+        <v>9123456734</v>
       </c>
       <c r="T5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="U5" t="s">
-        <v>83</v>
+        <v>61</v>
+      </c>
+      <c r="V5" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2023006</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="F6" s="1">
         <v>37413</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="H6">
         <v>121</v>
       </c>
       <c r="I6" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="M6">
         <v>9678901234</v>
       </c>
       <c r="N6" t="s">
-        <v>69</v>
+        <v>82</v>
+      </c>
+      <c r="P6" t="s">
+        <v>83</v>
       </c>
       <c r="Q6">
         <v>9123456900</v>
       </c>
+      <c r="R6">
+        <v>9123456999</v>
+      </c>
       <c r="T6" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="U6" t="s">
-        <v>84</v>
-      </c>
-      <c r="V6" s="1">
+        <v>35</v>
+      </c>
+      <c r="V6" t="s">
+        <v>85</v>
+      </c>
+      <c r="W6" s="1">
         <v>45077</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023007</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F7" s="1">
         <v>37079</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="H7">
         <v>130</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="J7" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="K7" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="L7" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="M7">
         <v>9789012345</v>
       </c>
       <c r="N7" t="s">
-        <v>78</v>
+        <v>94</v>
+      </c>
+      <c r="P7" t="s">
+        <v>95</v>
       </c>
       <c r="Q7">
         <v>9123456980</v>
       </c>
+      <c r="R7">
+        <v>9123456877</v>
+      </c>
       <c r="T7" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="U7" t="s">
-        <v>84</v>
-      </c>
-      <c r="V7" s="1">
+        <v>48</v>
+      </c>
+      <c r="V7" t="s">
+        <v>85</v>
+      </c>
+      <c r="W7" s="1">
         <v>45444</v>
       </c>
     </row>

</xml_diff>